<commit_message>
Update the base class to exclude creating the statvars for the columns that doesnt exists in the sheet. And added test cases.
</commit_message>
<xml_diff>
--- a/scripts/india_census/common/test_data/test_input.xlsx
+++ b/scripts/india_census/common/test_data/test_input.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="38">
   <si>
     <t xml:space="preserve">State</t>
   </si>
@@ -60,6 +60,24 @@
     <t xml:space="preserve">TOT_P</t>
   </si>
   <si>
+    <t xml:space="preserve">TOT_M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOT_F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_SC</t>
+  </si>
+  <si>
     <t xml:space="preserve">00</t>
   </si>
   <si>
@@ -94,6 +112,33 @@
   </si>
   <si>
     <t xml:space="preserve">JAMMU &amp; KASHMIR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISTRICT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kupwara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Badgam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leh(Ladakh)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kargil</t>
   </si>
 </sst>
 </file>
@@ -214,15 +259,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="942" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -260,34 +306,52 @@
       <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="J2" s="3" t="n">
         <v>249501663</v>
@@ -295,34 +359,52 @@
       <c r="K2" s="3" t="n">
         <v>1210854977</v>
       </c>
+      <c r="L2" s="3" t="n">
+        <v>623270258</v>
+      </c>
+      <c r="M2" s="3" t="n">
+        <v>587584719</v>
+      </c>
+      <c r="N2" s="3" t="n">
+        <v>164515253</v>
+      </c>
+      <c r="O2" s="3" t="n">
+        <v>85752254</v>
+      </c>
+      <c r="P2" s="3" t="n">
+        <v>78762999</v>
+      </c>
+      <c r="Q2" s="3" t="n">
+        <v>201378372</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="J3" s="3" t="n">
         <v>168612897</v>
@@ -330,34 +412,52 @@
       <c r="K3" s="3" t="n">
         <v>833748852</v>
       </c>
+      <c r="L3" s="3" t="n">
+        <v>427781058</v>
+      </c>
+      <c r="M3" s="3" t="n">
+        <v>405967794</v>
+      </c>
+      <c r="N3" s="3" t="n">
+        <v>121322865</v>
+      </c>
+      <c r="O3" s="3" t="n">
+        <v>63084449</v>
+      </c>
+      <c r="P3" s="3" t="n">
+        <v>58238416</v>
+      </c>
+      <c r="Q3" s="3" t="n">
+        <v>153850848</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="J4" s="3" t="n">
         <v>80888766</v>
@@ -365,34 +465,52 @@
       <c r="K4" s="3" t="n">
         <v>377106125</v>
       </c>
+      <c r="L4" s="3" t="n">
+        <v>195489200</v>
+      </c>
+      <c r="M4" s="3" t="n">
+        <v>181616925</v>
+      </c>
+      <c r="N4" s="3" t="n">
+        <v>43192388</v>
+      </c>
+      <c r="O4" s="3" t="n">
+        <v>22667805</v>
+      </c>
+      <c r="P4" s="3" t="n">
+        <v>20524583</v>
+      </c>
+      <c r="Q4" s="3" t="n">
+        <v>47527524</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>2119718</v>
@@ -400,34 +518,52 @@
       <c r="K5" s="0" t="n">
         <v>12541302</v>
       </c>
+      <c r="L5" s="0" t="n">
+        <v>6640662</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>5900640</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>2018905</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>1084355</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>934550</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>924991</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>1553433</v>
@@ -435,40 +571,659 @@
       <c r="K6" s="0" t="n">
         <v>9108060</v>
       </c>
+      <c r="L6" s="0" t="n">
+        <v>4774477</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>4333583</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>1593008</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>854141</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>738867</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>751026</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>566285</v>
       </c>
       <c r="K7" s="0" t="n">
         <v>3433242</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>1866185</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>1567057</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>425897</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>230214</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <v>195683</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>173965</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>113929</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>870354</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>474190</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>396164</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>188798</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>100459</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <v>88339</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>101930</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>765625</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>412038</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>353587</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>169588</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>90235</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <v>79353</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>11999</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>104729</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>62152</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>42577</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>19210</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>10224</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <v>8986</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>103363</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>753745</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>398041</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>355704</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>155202</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>84720</v>
+      </c>
+      <c r="P11" s="0" t="n">
+        <v>70482</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>89417</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>655833</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>343385</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>312448</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>140608</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>76753</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <v>63855</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>13946</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>97912</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>54656</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>43256</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>14594</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>7967</v>
+      </c>
+      <c r="P13" s="0" t="n">
+        <v>6627</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>21909</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>133487</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>78971</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <v>54516</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>12016</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>6174</v>
+      </c>
+      <c r="P14" s="0" t="n">
+        <v>5842</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>14905</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>87816</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>48411</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <v>39405</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>9053</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>4684</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <v>4369</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>7004</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>45671</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>30560</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <v>15111</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>2963</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>1490</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <v>1473</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>18338</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>140802</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>77785</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <v>63017</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>19928</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <v>10078</v>
+      </c>
+      <c r="P17" s="0" t="n">
+        <v>9850</v>
+      </c>
+      <c r="Q17" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>16147</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>124464</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <v>67703</v>
+      </c>
+      <c r="M18" s="0" t="n">
+        <v>56761</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <v>18359</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <v>9290</v>
+      </c>
+      <c r="P18" s="0" t="n">
+        <v>9069</v>
+      </c>
+      <c r="Q18" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -490,10 +1245,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -513,10 +1268,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>